<commit_message>
adding new fields in sale
</commit_message>
<xml_diff>
--- a/DailyReportTemplate1.xlsx
+++ b/DailyReportTemplate1.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,6 +460,10 @@
     <col width="20" customWidth="1" min="10" max="10"/>
     <col width="20" customWidth="1" min="11" max="11"/>
     <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1" ht="27" customHeight="1">
@@ -512,40 +516,57 @@
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
+          <t>SEAL NO</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
           <t>VOL OBS</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="K2" s="2" t="inlineStr">
         <is>
           <t>VOL 20</t>
         </is>
       </c>
-      <c r="K2" s="2" t="inlineStr">
+      <c r="L2" s="2" t="inlineStr">
         <is>
           <t>SELLING PRICE</t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
+      <c r="M2" s="2" t="inlineStr">
         <is>
           <t>PAYMENT</t>
+        </is>
+      </c>
+      <c r="N2" s="2" t="inlineStr">
+        <is>
+          <t>AMOUNT PAID</t>
+        </is>
+      </c>
+      <c r="O2" s="2" t="inlineStr">
+        <is>
+          <t>LOADING DATE</t>
+        </is>
+      </c>
+      <c r="P2" s="2" t="inlineStr">
+        <is>
+          <t>REMARKS</t>
         </is>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:P1"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation sqref="C3:C100000" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>=OFFSET('customers'!$A$1,0,0,COUNTA('customers'!$A:$A) - 0,1)</formula1>
     </dataValidation>
     <dataValidation sqref="B3:B100000" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"PMS,AGO,HFO,"</formula1>
     </dataValidation>
-    <dataValidation sqref="D3:D100000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>=OFFSET(trucks!$A$1,1, MATCH($C3, trucks!$A$1:$BY$1,0)-1,COUNTA(OFFSET(trucks!$A$1,1, MATCH($C3, trucks!$A$1:$BY$1,0)-1,200,1)),1)</formula1>
-    </dataValidation>
-    <dataValidation sqref="K3:K100000" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="M3:M100000" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"YES, NO"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
truck upload and modified date
</commit_message>
<xml_diff>
--- a/DailyReportTemplate1.xlsx
+++ b/DailyReportTemplate1.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="customers" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="trucks" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -580,7 +579,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A77"/>
+  <dimension ref="A1:A217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -591,993 +590,1519 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>WELLS OIL LIMITED</t>
+          <t>A. A. TRANSPORTERS</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>COLLUSSION  ENTERPRISES</t>
+          <t>ABUNDANT PETROLEUM</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>OAK ENERGY SOLUTUINS LTD</t>
+          <t>ACER PETROLEUM LIMITED</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PETRONEL SERVICES</t>
+          <t>ACO ENERGY</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CASREY</t>
+          <t>Adem Energy</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ONE PET</t>
+          <t>Africa gas &amp; Oil Co. Ltd (AGOL)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>AGRO CHEMICAL AND FOOD CO LIMITED</t>
+          <t>Afroasia Petroleum Company</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ALBA PETROLEUM LIMITED</t>
+          <t>AFTAH F SERVICES</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ALPHACHE SERVICES</t>
+          <t>AGRO CHEMICAL AND FOOD CO LIMITED</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ANDMORE ENTERPRISES LIMITED</t>
+          <t>ALBA PETROLEUM LIMITED</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BACHULAL POPATLAL K LTD</t>
+          <t>ALPHACHE SERVICES</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BAMBURI PORTLAND CEMENT LTD</t>
+          <t>ANDMORE ENTERPRISES LIMITED</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BELAN PETROLEUM LIMITED</t>
+          <t>ATTMAC</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BETAWAY PETROLEUM LIMITED</t>
+          <t>BACHULAL POPATLAL K LTD</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>BLUE SKY PETROLEUM</t>
+          <t>BAMBURI PORTLAND CEMENT LTD</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BORMAN ENTERPRISES LIMITED</t>
+          <t>BEAM ENERGY</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CANARY C AGENCY</t>
+          <t>BELAN PETROLEUM LIMITED</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DELTEX ENERGY</t>
+          <t>BELSA ENERGY LIMITED</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>DIESEL POWER</t>
+          <t>BENZENE SOLUTIONS LIMITED</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>DOANIC ENTERPRISE LTD</t>
+          <t>BEROWA TRADERS LIMITED</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>DULEXY ENTERPRISES</t>
+          <t>BETAWAY PETROLEUM LIMITED</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ELCOWING COMPANY LIMITED</t>
+          <t>BLUE OASIS VENTURES LTD</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>ELDORET PETROLEUM</t>
+          <t>BLUE SKY PETROLEUM</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ENSEN ENERGIES</t>
+          <t>BORMAN ENTERPRISES LIMITED</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>EON ENERGY LIMITED (FORMERLY SABILI)</t>
+          <t>BOTEG LIMITED</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>EQUITORIAL OILS</t>
+          <t>BRENTWOOD OIL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>FIFA HOLDINGS LIMITED</t>
+          <t>BRICARS AGENCIES</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>GALLANT FUEL ENTERPRISES</t>
+          <t>BROADWAY BAKERY LIMITED</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Gas Petro</t>
+          <t>BURAQ PETROLUM LIMITED</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t xml:space="preserve">GIKUSON </t>
+          <t>BUXTON PETROL STATION LIMITED</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>GOLDEN AFRICA KENYA LIMITED</t>
+          <t>CALSIF ENTERPRISES</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>GULF STREAM IINVESTMENTS LTD</t>
+          <t>CANARY C AGENCY</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>HASS PETROLEUM (K) LIMITED</t>
+          <t>CASREY</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>HEYINZ COMPANY LIMITED</t>
+          <t>CHEBEWOR FILLING STATION LTD</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>HEZDEP FUELS</t>
+          <t>CHEPNGESER TRADERS LTD</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>HILCONSAM ENTERPRISES</t>
+          <t>CHEV ENERGIES LTD</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>INC SUPPLIES LIMITED</t>
+          <t>China Civil Engineering Construction Corporation (K) LTD</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>JEMBO ENTERPRISES</t>
+          <t>COASTAL KENYA ENTERPRISES LTD</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>KEALSEY ENTERPRISES</t>
+          <t>COLLUSSION  ENTERPRISES</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>KENDRIE-EDGE ENTERPRISES LIMITED</t>
+          <t>CORRUGATED SHEETS LIMITED</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>KENSALT LIMITED</t>
+          <t>CROWN PETROLEUM LIMITED</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>KETTA GLOBAL INVESTMENT LTD</t>
+          <t>DELTEX ENERGY</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>KIMWAMUTU ENTERPRISE</t>
+          <t>DEPAR LTD</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>LEBOO COMPANY LIMITED</t>
+          <t>DEVKI STEEL MILLS LTD</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>LOKUTCH ENTERPRISES</t>
+          <t>DIESEL POWER</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>LORUK ENERGY</t>
+          <t>DISCOUNT FUELS LTD</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>MALEWA F STATION</t>
+          <t>DO NOT USE-FORMER GIL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>MANOA OIL (K) LTD</t>
+          <t>DOANIC ENTERPRISE LTD</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>MARANGO INVESTMENTS</t>
+          <t>DOLA PETROLEUM</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>MARS PETROLEUM</t>
+          <t>DOT CEE CONSTRUCTION LTD</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>MBTL</t>
+          <t>DREAMLINE EXPRESS</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>MILLY FRUITS</t>
+          <t>DRILMATIC ENGINEERING &amp;ENERGY LIMITED</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>MILLY GLASS</t>
+          <t>DULEXY ENTERPRISES</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>National Oil Corporation of KENYA Ltd</t>
+          <t>EAST AFRICAN ROADWAYS LTD</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>OBED PETROLEUM</t>
+          <t>EDIBLE OIL PRODUCTS LIMITED</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>OILMARK ENERGY LIMITED</t>
+          <t>ELCOWING COMPANY LIMITED</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>OLAM AVIV KENYA PRIVATE LIMITED</t>
+          <t>ELDORET PETROLEUM</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>QUICKFILL LTD</t>
+          <t>ENSEN ENERGIES</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t xml:space="preserve">RADHAN FILLING STATION LTD </t>
+          <t>EON ENERGY LIMITED (FORMERLY SABILI)</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>RADIANT EXPRESS SUPPLIES</t>
+          <t>EPPIC ENTERPRISES LIMITED</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>RAMJI HARIBHAI DEVANI</t>
+          <t>EPPIC OIL DO NOT USE</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>RANGERS OIL LIMITED</t>
+          <t>EQUITORIAL OILS</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>RESTOP ENERGY LIMITED</t>
+          <t>FANRIC TRADERS LIMITED</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>RICHFIELD SCION GLOBAL SOLUTIONS</t>
+          <t>FIFA HOLDINGS LIMITED</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>ROBAH LOGISTICS</t>
+          <t>FOCUS PREMIER LTD</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>ROYAL OIL COMPANY LIMITED</t>
+          <t>FRAJEM ENERGY</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>SAVA S STATION</t>
+          <t>FRANIC LIMITED</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>SHREEJI CHEMICALS LTD</t>
+          <t>GALLANT FUEL ENTERPRISES</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>SUMMER ENERGY LIMITED</t>
+          <t>Gas Petro</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>TALAI FILLING STATION</t>
+          <t>GEOSMART INVESTMENT CO LIMITED</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>TARMAL WIRE PRODUCTS LTD</t>
+          <t>GICOMU GAS LIMITED</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>TESCO MATT LIMITED</t>
+          <t xml:space="preserve">GIKUSON </t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>TOKYO (K) SERVICES</t>
+          <t>GOLD SPIKE CO LTD</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>TONONOKA ROLLING MILLS LTD</t>
+          <t>GOLDEN AFRICA KENYA LIMITED</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>TUNNEL INVESTMENT</t>
+          <t>Grain Bulk Handlers Limited</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>shs</t>
+          <t>GRAIN INDUSTRIES LTD</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>fd</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:BY5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+          <t>Grand Petroleum Station do not use</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>GREATMOUNT LPG LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>GULF STREAM IINVESTMENTS LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>HASS PETROLEUM (K) LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>HEMASON ENERGY</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>HEMAX VENTURES</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>HEYINZ COMPANY LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>HEZDEP FUELS</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>HEZDEP FUELS</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>HILCONSAM ENTERPRISES</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>HILWA PETROLEUM LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Hunkar Trading</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>INC SUPPLIES LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>JAFCOM KENYA LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>JEMBO ENTERPRISES</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>JIBCO KENYA LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>JOHN SMART</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>JOSMARK ENTERPRISES COMPANY LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>KAIBOS FILLING STATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>KAPSOIT FILLING STATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>KEALSEY ENTERPRISES</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>KENDAL ENERGY SOLUTIONS LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>KENDRIE-EDGE ENTERPRISES LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>KENODA S STATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>KENSALT LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>KENSOM ENERGY LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>KENTO ENERGY LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>KENYA ELECTRICITY GENERATING CO. PLC</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>KENYA RAILWAYS CORPORATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>KEROLITE PETROLEUM LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>KERRY GAS LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>KESTER PETROLEUM</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>KETTA GLOBAL INVESTMENT LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>KIMWAMUTU ENTERPRISE</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>KINAMBA S STATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>KLEAR MWIKI GAS SUPPLIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>KRAFT LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>LEBOO COMPANY LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>LEEK INVESTMENTS</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>LENSCO ENTERPRISES</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>LETTERMAN SUPPLIERS LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>LEXO ENERGY</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>LEYLAND PETROLEUM LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>LIDABA ENTERPRISES LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>LOKUTCH ENTERPRISES</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>LORI SYSTEMS LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>LORUK ENERGY</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Mackenzie Maritime (EA) Ltd</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>MAISHA MABATI MILLS LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>MAJESTIC PETROLEUM</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>MALEWA F STATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>MANASSE GICHUKI KURIA T/A DELTEX ENERGY</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>MANOA OIL (K) LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>MAPKA INVESTMENT LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>MAQBUL PETROLEUM LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>MARANGO INVESTMENTS</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>MARS PETROLEUM</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>MASS ENERGY (K) LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>MATECHA F STATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>MATUTA LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>MAX GAS AND PETROLEUM COMPANY LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>MBTL</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>MIDRIFT MERCHANT</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>MIDTOWN DEALERS LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>MILLY FRUITS</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>MILLY GLASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>MODERN COAST BUILDERS &amp; CONTRACTORS</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>MODERN COAST COACHES LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>MODERN TRUCKERS</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>MOMBASA CONTINENTAL RESORT</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>MOTREX LIMITED-MIKINDANI YARD</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>MOTREX LIMITED-VIPINGO YARD</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>MOTREX LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Mtawa S Station</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>MWANANCHI</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>NANDI HILLS</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>National Oil Corporation of KENYA Ltd</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>NEOKAWAN INVESTMENTS AND CONSORTIUM LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>NEW MEGA (AFRICA) LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>NOBIL S STATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>NYASINGA TRANSPORTERS</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>OAK ENERGY SOLUTUINS LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>OBED PETROLEUM</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>OILMARK ENERGY LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>OLAM AVIV KENYA PRIVATE LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>ONE PET</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>One petroleum -U Ltd</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Oxx Energy Limited</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>PADDY K LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>PETRONEL SERVICES</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>PLATOON INVESTMENT LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>POA ENERGY LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>PRESTIGE PREMIUM PETROLEUM LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>PROTO ENERGY LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>QUICKFILL LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RADHAN FILLING STATION LTD </t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>RADIANT EXPRESS SUPPLIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>RAMJI HARIBHAI DEVANI</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>RANGERS OIL LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>RASMI INTERNATIONAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>RAVAKO ENTERPRISES</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>RESTOP ENERGY LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>RICHFIELD SCION GLOBAL SOLUTIONS</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>ROBAH LOGISTICS</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>ROMBO PETROLEUM PRODUCT</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>ROYAL OIL COMPANY LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>SAVA S STATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>SEET INTERMOVERS</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>SEET TRADING COMPANY LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>SHREEJI CHEMICALS LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>SHREEJI ENTERPRISES K LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>SIPREMA OIL COMPANY LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>SMOOTHRIFT MERCHANTS</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Solution E.A Ltd</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>SPECTA ENERGY LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>STARWAY INTERNATIONAL FREIGHT AND FORWARDERS LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>SUMMER ENERGY LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>SWAN CARRIERS LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>SWIFT ENERGY DISTRIBUTERS LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>TALAI FILLING STATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>TARMAL WIRE PRODUCTS LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>TESCO MATT LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>TEX TRADING</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>TEXAS SERVICE STATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>THIKA PETROLEUM LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>TIGER OIL LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>TOGAN TRANSPORTERS</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>TOKYO (K) SERVICES</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>TONONOKA ROLLING MILLS LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>TOPGAS TRADERS EA LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>TOPLINE TRADERS LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>TOTAL LINK LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>Toyo Construction Company</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>Toyo Construction Company</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>TRIPLE EIGHT TRANSPORTERS</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>TUNNEL INVESTMENT</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>VIKI ENERGY LIMITED</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
         <is>
           <t>WELLS OIL LIMITED</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>COLLUSSION  ENTERPRISES</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>OAK ENERGY SOLUTUINS LTD</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>PETRONEL SERVICES</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>CASREY</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>ONE PET</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>AGRO CHEMICAL AND FOOD CO LIMITED</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>ALBA PETROLEUM LIMITED</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>ALPHACHE SERVICES</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>ANDMORE ENTERPRISES LIMITED</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>BACHULAL POPATLAL K LTD</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>BAMBURI PORTLAND CEMENT LTD</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>BELAN PETROLEUM LIMITED</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>BETAWAY PETROLEUM LIMITED</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>BLUE SKY PETROLEUM</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>BORMAN ENTERPRISES LIMITED</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>CANARY C AGENCY</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>DELTEX ENERGY</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>DIESEL POWER</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>DOANIC ENTERPRISE LTD</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>DULEXY ENTERPRISES</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>ELCOWING COMPANY LIMITED</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>ELDORET PETROLEUM</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>ENSEN ENERGIES</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>EON ENERGY LIMITED (FORMERLY SABILI)</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>EQUITORIAL OILS</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>FIFA HOLDINGS LIMITED</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>GALLANT FUEL ENTERPRISES</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>Gas Petro</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">GIKUSON </t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>GOLDEN AFRICA KENYA LIMITED</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>GULF STREAM IINVESTMENTS LTD</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>HASS PETROLEUM (K) LIMITED</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>HEYINZ COMPANY LIMITED</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>HEZDEP FUELS</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>HILCONSAM ENTERPRISES</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>INC SUPPLIES LIMITED</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>JEMBO ENTERPRISES</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>KEALSEY ENTERPRISES</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>KENDRIE-EDGE ENTERPRISES LIMITED</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>KENSALT LIMITED</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>KETTA GLOBAL INVESTMENT LTD</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>KIMWAMUTU ENTERPRISE</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>LEBOO COMPANY LIMITED</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>LOKUTCH ENTERPRISES</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>LORUK ENERGY</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>MALEWA F STATION</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>MANOA OIL (K) LTD</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>MARANGO INVESTMENTS</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>MARS PETROLEUM</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>MBTL</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>MILLY FRUITS</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>MILLY GLASS</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>National Oil Corporation of KENYA Ltd</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>OBED PETROLEUM</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>OILMARK ENERGY LIMITED</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>OLAM AVIV KENYA PRIVATE LIMITED</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>QUICKFILL LTD</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RADHAN FILLING STATION LTD </t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>RADIANT EXPRESS SUPPLIES</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>RAMJI HARIBHAI DEVANI</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>RANGERS OIL LIMITED</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>RESTOP ENERGY LIMITED</t>
-        </is>
-      </c>
-      <c r="BL1" t="inlineStr">
-        <is>
-          <t>RICHFIELD SCION GLOBAL SOLUTIONS</t>
-        </is>
-      </c>
-      <c r="BM1" t="inlineStr">
-        <is>
-          <t>ROBAH LOGISTICS</t>
-        </is>
-      </c>
-      <c r="BN1" t="inlineStr">
-        <is>
-          <t>ROYAL OIL COMPANY LIMITED</t>
-        </is>
-      </c>
-      <c r="BO1" t="inlineStr">
-        <is>
-          <t>SAVA S STATION</t>
-        </is>
-      </c>
-      <c r="BP1" t="inlineStr">
-        <is>
-          <t>SHREEJI CHEMICALS LTD</t>
-        </is>
-      </c>
-      <c r="BQ1" t="inlineStr">
-        <is>
-          <t>SUMMER ENERGY LIMITED</t>
-        </is>
-      </c>
-      <c r="BR1" t="inlineStr">
-        <is>
-          <t>TALAI FILLING STATION</t>
-        </is>
-      </c>
-      <c r="BS1" t="inlineStr">
-        <is>
-          <t>TARMAL WIRE PRODUCTS LTD</t>
-        </is>
-      </c>
-      <c r="BT1" t="inlineStr">
-        <is>
-          <t>TESCO MATT LIMITED</t>
-        </is>
-      </c>
-      <c r="BU1" t="inlineStr">
-        <is>
-          <t>TOKYO (K) SERVICES</t>
-        </is>
-      </c>
-      <c r="BV1" t="inlineStr">
-        <is>
-          <t>TONONOKA ROLLING MILLS LTD</t>
-        </is>
-      </c>
-      <c r="BW1" t="inlineStr">
-        <is>
-          <t>TUNNEL INVESTMENT</t>
-        </is>
-      </c>
-      <c r="BX1" t="inlineStr">
-        <is>
-          <t>shs</t>
-        </is>
-      </c>
-      <c r="BY1" t="inlineStr">
-        <is>
-          <t>fd</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>plate_no</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>KCV 5674</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>KBC 3487</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>kbc 3457</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>kbv 5676</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>kbv</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>new</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>yt</t>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>WHITE HORSE CARRIERS LTD</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>WILLONES ENERGY</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>YABALO LOGISTICS-SMC LIMITED</t>
         </is>
       </c>
     </row>

</xml_diff>